<commit_message>
Punto 1 final y avance 2
</commit_message>
<xml_diff>
--- a/output/resultados_regresiones.xlsx
+++ b/output/resultados_regresiones.xlsx
@@ -20,13 +20,13 @@
     <t xml:space="preserve">.stat</t>
   </si>
   <si>
-    <t xml:space="preserve">Model 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model 3</t>
+    <t xml:space="preserve">Modelo 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo 3</t>
   </si>
   <si>
     <t xml:space="preserve">(Intercept)</t>
@@ -38,10 +38,10 @@
     <t xml:space="preserve">-174809474.238***</t>
   </si>
   <si>
-    <t xml:space="preserve">-394911554.937***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-242797669.349***</t>
+    <t xml:space="preserve">-177063223.674***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-69043404.727***</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -53,10 +53,10 @@
     <t xml:space="preserve">[7127105.314]</t>
   </si>
   <si>
-    <t xml:space="preserve">[9557369.872]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[11014206.342]</t>
+    <t xml:space="preserve">[7052644.424]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8127293.665]</t>
   </si>
   <si>
     <t xml:space="preserve">rooms</t>
@@ -122,13 +122,13 @@
     <t xml:space="preserve">[21726.583]</t>
   </si>
   <si>
-    <t xml:space="preserve">tipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">217848331.263***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">173754264.622***</t>
+    <t xml:space="preserve">as.factor(property_type)Casa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-217848331.263***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-173754264.622***</t>
   </si>
   <si>
     <t xml:space="preserve">[6384368.197]</t>

</xml_diff>